<commit_message>
Added LEO, including onsite emissions for stationary NG combustion at the facility
</commit_message>
<xml_diff>
--- a/input_fuel_pathway_data/CRF_calcs.xlsx
+++ b/input_fuel_pathway_data/CRF_calcs.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danikamacdonell/Git/MIT_NavigaTE_inputs/input_fuel_pathway_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{85D2D4B9-EA1B-9648-B2F9-89339D789AC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F2C0856-463A-FF41-AF8D-4A681BBCDB5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15780" xr2:uid="{84662608-0ADE-2D4E-859D-A4755BFAA688}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,28 +38,14 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={22802913-BB14-3B4F-9C0F-984A1CC0F922}</author>
-    <author>tc={D252ACC2-1F6A-F44B-A5CC-F7CC1ABDE63A}</author>
     <author>tc={0869BFCE-344E-5B43-A202-E221F7463EA1}</author>
+    <author>tc={0E1CAFE1-F32B-CF46-AC91-2ED6B02887D5}</author>
+    <author>tc={D67E13D9-C8DC-C445-934F-34F915302587}</author>
+    <author>tc={EEC0881D-7366-9C4E-9546-425A7DFA3499}</author>
+    <author>tc={2CDC5AE4-6E39-884D-AF86-075B7899AC4C}</author>
   </authors>
   <commentList>
-    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{22802913-BB14-3B4F-9C0F-984A1CC0F922}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Calculated using Fisher equation: https://corporatefinanceinstitute.com/resources/economics/fisher-equation/</t>
-      </text>
-    </comment>
-    <comment ref="K3" authorId="1" shapeId="0" xr:uid="{D252ACC2-1F6A-F44B-A5CC-F7CC1ABDE63A}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Calculated using Fisher equation: https://corporatefinanceinstitute.com/resources/economics/fisher-equation/</t>
-      </text>
-    </comment>
-    <comment ref="A4" authorId="2" shapeId="0" xr:uid="{0869BFCE-344E-5B43-A202-E221F7463EA1}">
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{0869BFCE-344E-5B43-A202-E221F7463EA1}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -67,28 +53,48 @@
     Data obtained from Table 5 in Zang et al (https://www.sciencedirect.com/science/article/abs/pii/S0360319923048760)</t>
       </text>
     </comment>
+    <comment ref="A5" authorId="1" shapeId="0" xr:uid="{0E1CAFE1-F32B-CF46-AC91-2ED6B02887D5}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Data obtained from Table S2 of https://www.sciencedirect.com/science/article/abs/pii/S0360319923048760</t>
+      </text>
+    </comment>
+    <comment ref="A6" authorId="2" shapeId="0" xr:uid="{D67E13D9-C8DC-C445-934F-34F915302587}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    From Table S4 on Pg. S11 of https://pubs.acs.org/doi/suppl/10.1021/acs.est.2c03960/suppl_file/es2c03960_si_001.pdf</t>
+      </text>
+    </comment>
+    <comment ref="B6" authorId="3" shapeId="0" xr:uid="{EEC0881D-7366-9C4E-9546-425A7DFA3499}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    From Table ES-2 in https://docs.nrel.gov/docs/fy15osti/62455.pdf</t>
+      </text>
+    </comment>
+    <comment ref="C6" authorId="4" shapeId="0" xr:uid="{2CDC5AE4-6E39-884D-AF86-075B7899AC4C}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    From Table 1 on pg. 5 of https://docs.nrel.gov/docs/fy15osti/62455.pdf</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>H2_ATRCCS</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">After-tax Real IRR (%) </t>
   </si>
   <si>
-    <t xml:space="preserve">Inflation rate (%) </t>
-  </si>
-  <si>
-    <t>nominal discount rate</t>
-  </si>
-  <si>
-    <t>Plant life (years)</t>
-  </si>
-  <si>
     <t>CRF</t>
   </si>
   <si>
@@ -98,14 +104,23 @@
     <t>Pathway</t>
   </si>
   <si>
-    <t>Bio-CFP</t>
+    <t>NG Liquefaction</t>
+  </si>
+  <si>
+    <t>Depreciation Recovery period (years)</t>
+  </si>
+  <si>
+    <t>H2_*</t>
+  </si>
+  <si>
+    <t>CFP and LEO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -134,8 +149,8 @@
     </font>
     <font>
       <sz val="12"/>
-      <name val="Aptos Narrow"/>
-      <scheme val="minor"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos"/>
     </font>
   </fonts>
   <fills count="2">
@@ -503,24 +518,6 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="D3" dT="2025-08-17T05:20:10.17" personId="{04B2AFC0-242F-F043-8052-59A4060FF714}" id="{22802913-BB14-3B4F-9C0F-984A1CC0F922}">
-    <text>Calculated using Fisher equation: https://corporatefinanceinstitute.com/resources/economics/fisher-equation/</text>
-    <extLst>
-      <x:ext xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" uri="{F7C98A9C-CBB3-438F-8F68-D28B6AF4A901}">
-        <xltc2:checksum>992724882</xltc2:checksum>
-        <xltc2:hyperlink startIndex="34" length="74" url="https://corporatefinanceinstitute.com/resources/economics/fisher-equation/"/>
-      </x:ext>
-    </extLst>
-  </threadedComment>
-  <threadedComment ref="K3" dT="2025-08-17T05:20:10.17" personId="{04B2AFC0-242F-F043-8052-59A4060FF714}" id="{D252ACC2-1F6A-F44B-A5CC-F7CC1ABDE63A}">
-    <text>Calculated using Fisher equation: https://corporatefinanceinstitute.com/resources/economics/fisher-equation/</text>
-    <extLst>
-      <x:ext xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" uri="{F7C98A9C-CBB3-438F-8F68-D28B6AF4A901}">
-        <xltc2:checksum>992724882</xltc2:checksum>
-        <xltc2:hyperlink startIndex="34" length="74" url="https://corporatefinanceinstitute.com/resources/economics/fisher-equation/"/>
-      </x:ext>
-    </extLst>
-  </threadedComment>
   <threadedComment ref="A4" dT="2025-08-17T05:22:23.60" personId="{04B2AFC0-242F-F043-8052-59A4060FF714}" id="{0869BFCE-344E-5B43-A202-E221F7463EA1}">
     <text>Data obtained from Table 5 in Zang et al (https://www.sciencedirect.com/science/article/abs/pii/S0360319923048760)</text>
     <extLst>
@@ -530,111 +527,138 @@
       </x:ext>
     </extLst>
   </threadedComment>
+  <threadedComment ref="A5" dT="2025-08-17T21:45:20.05" personId="{04B2AFC0-242F-F043-8052-59A4060FF714}" id="{0E1CAFE1-F32B-CF46-AC91-2ED6B02887D5}">
+    <text>Data obtained from Table S2 of https://www.sciencedirect.com/science/article/abs/pii/S0360319923048760</text>
+    <extLst>
+      <x:ext xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" uri="{F7C98A9C-CBB3-438F-8F68-D28B6AF4A901}">
+        <xltc2:checksum>552084019</xltc2:checksum>
+        <xltc2:hyperlink startIndex="31" length="71" url="https://www.sciencedirect.com/science/article/abs/pii/S0360319923048760"/>
+      </x:ext>
+    </extLst>
+  </threadedComment>
+  <threadedComment ref="A6" dT="2025-08-18T20:42:35.95" personId="{04B2AFC0-242F-F043-8052-59A4060FF714}" id="{D67E13D9-C8DC-C445-934F-34F915302587}">
+    <text>From Table S4 on Pg. S11 of https://pubs.acs.org/doi/suppl/10.1021/acs.est.2c03960/suppl_file/es2c03960_si_001.pdf</text>
+    <extLst>
+      <x:ext xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" uri="{F7C98A9C-CBB3-438F-8F68-D28B6AF4A901}">
+        <xltc2:checksum>3728333554</xltc2:checksum>
+        <xltc2:hyperlink startIndex="28" length="86" url="https://pubs.acs.org/doi/suppl/10.1021/acs.est.2c03960/suppl_file/es2c03960_si_001.pdf"/>
+      </x:ext>
+    </extLst>
+  </threadedComment>
+  <threadedComment ref="B6" dT="2025-08-17T22:02:39.31" personId="{04B2AFC0-242F-F043-8052-59A4060FF714}" id="{EEC0881D-7366-9C4E-9546-425A7DFA3499}">
+    <text>From Table ES-2 in https://docs.nrel.gov/docs/fy15osti/62455.pdf</text>
+    <extLst>
+      <x:ext xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" uri="{F7C98A9C-CBB3-438F-8F68-D28B6AF4A901}">
+        <xltc2:checksum>624118638</xltc2:checksum>
+        <xltc2:hyperlink startIndex="19" length="45" url="https://docs.nrel.gov/docs/fy15osti/62455.pdf"/>
+      </x:ext>
+    </extLst>
+  </threadedComment>
+  <threadedComment ref="C6" dT="2025-08-17T22:02:14.60" personId="{04B2AFC0-242F-F043-8052-59A4060FF714}" id="{2CDC5AE4-6E39-884D-AF86-075B7899AC4C}">
+    <text>From Table 1 on pg. 5 of https://docs.nrel.gov/docs/fy15osti/62455.pdf</text>
+    <extLst>
+      <x:ext xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" uri="{F7C98A9C-CBB3-438F-8F68-D28B6AF4A901}">
+        <xltc2:checksum>1772361740</xltc2:checksum>
+        <xltc2:hyperlink startIndex="25" length="45" url="https://docs.nrel.gov/docs/fy15osti/62455.pdf"/>
+      </x:ext>
+    </extLst>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A57E614A-2C83-E448-83DC-69AAC29D7EC4}">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B1" s="1"/>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2">
         <v>8</v>
       </c>
       <c r="C4" s="2">
+        <v>20</v>
+      </c>
+      <c r="D4" s="2">
+        <f>B4/100*(1+B4/100)^C4/((1+B4/100)^C4-1)</f>
+        <v>0.10185220882315059</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="3">
-        <f>(1+B4/100)*(1+C4/100)-1</f>
-        <v>0.10160000000000013</v>
-      </c>
-      <c r="E4" s="2">
-        <v>40</v>
-      </c>
-      <c r="F4" s="2">
-        <f>D4*(1+D4)^E4/((1+D4)^E4-1)</f>
-        <v>0.10376314705751892</v>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>20</v>
+      </c>
+      <c r="D5" s="2">
+        <f>B5/100*(1+B5/100)^C5/((1+B5/100)^C5-1)</f>
+        <v>0.11745962477254576</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>8</v>
-      </c>
-      <c r="C5">
-        <v>1.9</v>
-      </c>
-      <c r="D5" s="3">
-        <f>(1+B5/100)*(1+C5/100)-1</f>
-        <v>0.10051999999999994</v>
-      </c>
-      <c r="E5">
-        <v>40</v>
-      </c>
-      <c r="F5" s="2">
-        <f>D5*(1+D5)^E5/((1+D5)^E5-1)</f>
-        <v>0.10274768859314053</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>10</v>
       </c>
       <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6" s="3">
-        <f>(1+B6/100)*(1+C6/100)-1</f>
-        <v>0.12200000000000011</v>
-      </c>
-      <c r="E6">
-        <v>30</v>
-      </c>
-      <c r="F6" s="2">
-        <f>D6*(1+D6)^E6/((1+D6)^E6-1)</f>
-        <v>0.12598599322823506</v>
+        <v>20</v>
+      </c>
+      <c r="D6" s="2">
+        <f>B6/100*(1+B6/100)^C6/((1+B6/100)^C6-1)</f>
+        <v>0.11745962477254576</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>20</v>
+      </c>
+      <c r="D7" s="2">
+        <f>B7/100*(1+B7/100)^C7/((1+B7/100)^C7-1)</f>
+        <v>0.10185220882315059</v>
       </c>
     </row>
   </sheetData>

</xml_diff>